<commit_message>
Refreshed tumor stage analysis
</commit_message>
<xml_diff>
--- a/DGEA/Union/Gene_overlap.xlsx
+++ b/DGEA/Union/Gene_overlap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
   <si>
     <t>Comparison</t>
   </si>
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,7 +563,9 @@
       <c r="E4" s="5">
         <v>11437</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7">
+        <v>10249</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
@@ -581,7 +583,9 @@
       <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7">
+        <v>9537</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -593,8 +597,12 @@
       <c r="C6" s="3">
         <v>8045</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="3">
+        <v>10249</v>
+      </c>
+      <c r="E6" s="3">
+        <v>9537</v>
+      </c>
       <c r="F6" s="4" t="s">
         <v>5</v>
       </c>
@@ -607,12 +615,140 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8">
+        <v>10891</v>
+      </c>
+      <c r="D2" s="8">
+        <v>16191</v>
+      </c>
+      <c r="E2" s="8">
+        <v>12934</v>
+      </c>
+      <c r="F2" s="10">
+        <v>11512</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>10891</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5">
+        <v>10621</v>
+      </c>
+      <c r="E3" s="5">
+        <v>8597</v>
+      </c>
+      <c r="F3" s="7">
+        <v>8045</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
+        <v>16191</v>
+      </c>
+      <c r="C4" s="5">
+        <v>10621</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5">
+        <v>11437</v>
+      </c>
+      <c r="F4" s="7">
+        <v>10249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <v>12934</v>
+      </c>
+      <c r="C5" s="5">
+        <v>8597</v>
+      </c>
+      <c r="D5" s="5">
+        <v>11437</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="7">
+        <v>9537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9">
+        <v>11512</v>
+      </c>
+      <c r="C6" s="3">
+        <v>8045</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10249</v>
+      </c>
+      <c r="E6" s="3">
+        <v>9537</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>